<commit_message>
Tenta corrigir erro 3
Números desfortados - tentativa de consertá-los
</commit_message>
<xml_diff>
--- a/upload/despesa-pessoal-acordo-judicial-brumadinho.xlsx
+++ b/upload/despesa-pessoal-acordo-judicial-brumadinho.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28412"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13F6FE39-17FD-4E93-B5E8-9162807BB802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C40AC88-2541-45CB-8F76-89400E6DF188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,34 +33,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12269" uniqueCount="285">
   <si>
-    <t>Ano_Mês</t>
+    <t>ano_mes</t>
   </si>
   <si>
-    <t>MASP</t>
+    <t>masp</t>
   </si>
   <si>
-    <t>Orgão_sigla</t>
+    <t>orgao_sigla</t>
   </si>
   <si>
-    <t>Órgão</t>
+    <t>orgao</t>
   </si>
   <si>
-    <t>Nome</t>
+    <t>nome</t>
   </si>
   <si>
-    <t>Valor</t>
+    <t>valor</t>
   </si>
   <si>
-    <t>Cargo_sigla</t>
+    <t>cargo_sigla</t>
   </si>
   <si>
-    <t>Cargo_descrição</t>
+    <t>cargo_descricao</t>
   </si>
   <si>
-    <t>Data_início_contrato</t>
+    <t>data_inicio_contrato</t>
   </si>
   <si>
-    <t>Data_término_contrato</t>
+    <t>data_termino_contrato</t>
   </si>
   <si>
     <t>Secretaria de Estado de Saúde</t>
@@ -1260,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2441"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A2435" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F2441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1294,10 +1294,10 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>